<commit_message>
adding new actor to use case and add new use case to the diagram, also fixing spelling on G16_Acceptence file
</commit_message>
<xml_diff>
--- a/system design/G16_Acceptance.xlsx
+++ b/system design/G16_Acceptance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreibeloziorove/Desktop/middleProjectBistro_16/system design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F43DEAD-DCB4-5147-9B98-8444A6613B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9743362-64A1-E540-9381-12CA09A11000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15220" yWindow="880" windowWidth="14820" windowHeight="18560" xr2:uid="{DACF97BE-494E-BD4D-8128-8A3419E5BFA1}"/>
+    <workbookView xWindow="200" yWindow="880" windowWidth="29840" windowHeight="18560" xr2:uid="{DACF97BE-494E-BD4D-8128-8A3419E5BFA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t xml:space="preserve">The system will allow you to connect through a terminal in the restaurant </t>
   </si>
   <si>
-    <t>The booking windows were half an hour apart</t>
-  </si>
-  <si>
     <t>The Place an Order window will be within an hour to a month from the date an order is created</t>
   </si>
   <si>
@@ -86,15 +83,9 @@
     <t>Offer a ceiling space if there is no available space at the time the customer wants or there is no available table of the size he wants</t>
   </si>
   <si>
-    <t>Close times are in the same sea from the range of an hour to the closing of a restaurant on the same day</t>
-  </si>
-  <si>
     <t xml:space="preserve">The system will allow you to send a reminder to the customer </t>
   </si>
   <si>
-    <t>The reminder will be via SMS or e-mail</t>
-  </si>
-  <si>
     <t>Automatic cancellation of an order will be made 15 minutes after a customer is late for their order</t>
   </si>
   <si>
@@ -162,6 +153,15 @@
   </si>
   <si>
     <t>NFR</t>
+  </si>
+  <si>
+    <t>Each booking window will have half an hour apart</t>
+  </si>
+  <si>
+    <t>Close times are in the same day from the range of an hour to the closing of a restaurant on the same day</t>
+  </si>
+  <si>
+    <t>The reminder will be sent via SMS or e-mail</t>
   </si>
 </sst>
 </file>
@@ -616,8 +616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527762F5-D11B-D449-919A-74259918E4FE}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="239" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="43.5" defaultRowHeight="73" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -628,13 +628,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -645,7 +645,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -657,7 +657,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -669,7 +669,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -680,7 +680,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -691,7 +691,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -702,7 +702,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -713,7 +713,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -724,7 +724,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -735,7 +735,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -743,10 +743,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -754,10 +754,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -765,10 +765,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -776,10 +776,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -787,10 +787,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -798,10 +798,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -809,10 +809,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -820,10 +820,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -831,10 +831,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -842,10 +842,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -853,10 +853,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -864,10 +864,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -875,10 +875,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -886,10 +886,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -897,10 +897,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -908,10 +908,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -919,10 +919,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -930,10 +930,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -941,10 +941,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -952,10 +952,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -963,10 +963,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -974,10 +974,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -985,10 +985,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -996,10 +996,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -1007,10 +1007,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C35" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -1018,10 +1018,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -1029,10 +1029,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -1040,10 +1040,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding acceptence test for the Ordering functainality in the system
</commit_message>
<xml_diff>
--- a/system design/G16_Acceptance.xlsx
+++ b/system design/G16_Acceptance.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreibeloziorove/Desktop/middleProjectBistro_16/system design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9743362-64A1-E540-9381-12CA09A11000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A18E89D-0190-254C-B58D-565699814E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="880" windowWidth="29840" windowHeight="18560" xr2:uid="{DACF97BE-494E-BD4D-8128-8A3419E5BFA1}"/>
+    <workbookView xWindow="1340" yWindow="820" windowWidth="67260" windowHeight="27780" activeTab="1" xr2:uid="{DACF97BE-494E-BD4D-8128-8A3419E5BFA1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="requirments" sheetId="1" r:id="rId1"/>
+    <sheet name="Acceptence test Ordering " sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
   <si>
     <t>The system will allow you to register subscribers to the system</t>
   </si>
@@ -162,13 +163,386 @@
   </si>
   <si>
     <t>The reminder will be sent via SMS or e-mail</t>
+  </si>
+  <si>
+    <t>Test ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Precondition</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The system will allow to remote connection </t>
+  </si>
+  <si>
+    <t>the system will allow to connect via terminal</t>
+  </si>
+  <si>
+    <t>remoteConnectSuccseful</t>
+  </si>
+  <si>
+    <t>customer want to connect to system coustumer open the GUI (web/application).
+Custumer click "start".
+ The customer attempt to connect to the system.</t>
+  </si>
+  <si>
+    <t>the system try to connect to the server. 
+The application connect via internet to the backend server.
+Backend will make connection with the frontend. 
+The server sent to the GUI that the connection sucssesful
+the GUI will show to the user "connection sucssesful"</t>
+  </si>
+  <si>
+    <t>the backend server need to be online 
+the backend server need to be accessible</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>OrderSubscriberSuccsesful</t>
+  </si>
+  <si>
+    <t>the subscriver want to make resurvation to resturant.
+The subscriber try to make auth,
+select date
+selsct time
+select number of guests
+and click order</t>
+  </si>
+  <si>
+    <t>the system will allow to scan confirmation code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the system will allow to scan QR code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the QR code can work as conforamtion code </t>
+  </si>
+  <si>
+    <t>the system connect to DB to sub table and check if the auth of the subscriber is valid 
+after that the system get Ordering requsest for reserving table. The system check in the DB if there is in this date, in that time for this amount of guests table.
+the system find that there is table 
+the system accept the Order and write it to the DB.
+the system sent to subscriber "confomation code" of the reservation table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the subscriber is aleady in the system
+there is table in that datetime in currect size </t>
+  </si>
+  <si>
+    <t xml:space="preserve">none </t>
+  </si>
+  <si>
+    <t>the test fail because the user is not give all the information like don’t give time.</t>
+  </si>
+  <si>
+    <t>the subscriver want to make resurvation to resturant.
+The subscriber try to make auth,
+select date
+select number of guests
+and click order</t>
+  </si>
+  <si>
+    <t>OrderSubscriberNotGiveTimeFail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the subscriber is aleady in the system
+the DB is accessble
+there is table in that datetime in currect size </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the system connect to DB to sub table and check if the auth of the subscriber is valid 
+the GUI before sending Ordering request to the server check if all the fields was filled with data. 
+After the check the fields the GUI sent messege to the user that the "time field is emplty" </t>
+  </si>
+  <si>
+    <t>the subscriver want to make resurvation to resturant.
+The subscriber try to make auth,
+select date
+select time 
+select number of guests
+and click order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the system connect to DB to sub table and check if the auth of the subscriber is valid 
+after that the system get Ordering requsest for reserving table. The system check in the DB if time jump is valid 
+The system find that the time jump isn't valid
+the system is sent responce to the sub that: "the time jump isn't correct you can order only in  in hulf hour jump"
+</t>
+  </si>
+  <si>
+    <t>OrderSubscriberNotValidJumpTimeFail</t>
+  </si>
+  <si>
+    <t>OrderSubscriberTimeOneHourLessFail</t>
+  </si>
+  <si>
+    <t>the test fail because the user is give not valid jump of the time it can be in full hour like 15:00 or in hulf hour like 17:30</t>
+  </si>
+  <si>
+    <t>the subscriver want to make resurvation to resturant.
+The subscriber try to make auth,
+select date
+select time (less then hour)
+select number of guests
+and click order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the test fail because the user is give not valid time less the hour to from the Ordering time. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the system connect to DB to sub table and check if the auth of the subscriber is valid 
+after that the system get Ordering requsest for reserving table. The system check in the DB if time is valid 
+The system find that the time of oegring is less then the ordering moment:  isn't valid
+the system is sent responce to the sub that: "the time isn't correct cant order for this time. too close"
+</t>
+  </si>
+  <si>
+    <t>OrderSubscriberTooFarFail</t>
+  </si>
+  <si>
+    <t>the subscriver want to make resurvation to resturant.
+The subscriber try to make auth,
+select date (two months from the order time )
+select time 
+select number of guests
+and click order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the system connect to DB to sub table and check if the auth of the subscriber is valid 
+after that the system get Ordering requsest for reserving table. The system check in the DB if date is valid 
+The system find that the date of ordering is too far, more then one month then the ordering moment:  isn't valid
+the system is sent responce to the sub that: "the time isn't correct cant order for this date. too far"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the test fail because the user is give not valid date of the order besouse it too far from the max date limit. (one month) </t>
+  </si>
+  <si>
+    <t>OrderSubscriberTooMuchGuestsFail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the system connect to DB to sub table and check if the auth of the subscriber is valid 
+after that the system get Ordering requsest for reserving table. The system check in the DB if there is table in that size 
+The system find that the there is no that big table in the resturant
+the system is sent responce to the sub that: "can't reserve palce to that much of people, you hit the limit of the biggest table (max 10)"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the test check if the system can find if the limit of the tables and sent response that it too much for one order. </t>
+  </si>
+  <si>
+    <t>the subscriner want to make resurvation to resturant.
+The subscriber try to make auth,
+select date 
+select time 
+select number of guests (number of gusts is bigger then the max table)
+and click order</t>
+  </si>
+  <si>
+    <t>OrderSubscriberNoTableAviableInThatSizeFail</t>
+  </si>
+  <si>
+    <t>the subscriner want to make resurvation to resturant.
+The subscriber try to make auth,
+select date 
+select time 
+select number of guests 
+and click order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the system connect to DB to sub table and check if the auth of the subscriber is valid 
+after that the system get Ordering requsest for reserving table. The system check in the DB if there is table in that size aviable in that time  
+The system find that the all tables in that size all capture.
+the system is sent responce to the sub that: "can't reserve palce to that much of people, all the tables capable to hold this reservation already capture"
+</t>
+  </si>
+  <si>
+    <t>the test check if the system can find if the limit of the tables and sent response that all the match tables are acupide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the subscriber is aleady in the system
+the DB is accessble
+there is table empty 
+the number of goust bigger then the max size table
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the subscriber is aleady in the system
+the DB is accessble
+there is table empty
+all the table in that size of order are already acupide by other Orders 
+</t>
+  </si>
+  <si>
+    <t>OrderCasualCustomerSuccsesful</t>
+  </si>
+  <si>
+    <t>OrderCasualCustomerNotGiveTimeFail</t>
+  </si>
+  <si>
+    <t>OrderCasualCustomerNotValidJumpTimeFail</t>
+  </si>
+  <si>
+    <t>OrderCasualCustomerTimeOneHourLessFail</t>
+  </si>
+  <si>
+    <t>OrderCasualCustomerTooFarFail</t>
+  </si>
+  <si>
+    <t>OrderCasualCustomerTooMuchGuestsFail</t>
+  </si>
+  <si>
+    <t>OrderCasualCustomerNoTableAviableInThatSizeFail</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The system check in the DB if there is in this date, in that time for this amount of guests table.
+the system find that there is table 
+the system accept the Order and write it to the DB.
+the system sent to subscriber "confomation code" of the reservation table</t>
+  </si>
+  <si>
+    <t>the Casual customer want to make resurvation to resturant.
+select date
+selsct time
+select number of guests,
+write telepone number / Email
+and click order</t>
+  </si>
+  <si>
+    <t>the Casual customer want to make resurvation to resturant.
+select date
+select number of guests
+write telepone number / Email
+and click order</t>
+  </si>
+  <si>
+    <t>the Casual customer want to make resurvation to resturant.
+select date
+select time 
+select number of guests
+write telepone number / Email
+and click order</t>
+  </si>
+  <si>
+    <t>the Casual customer want to make resurvation to resturant.
+select date
+select time (less then hour)
+select number of guests
+write telepone number / Email
+and click order</t>
+  </si>
+  <si>
+    <t>the Casual customer want to make resurvation to resturant.
+select date (two months from the order time )
+select time 
+select number of guests
+write telepone number / Email
+and click order</t>
+  </si>
+  <si>
+    <t>the Casual customer want to make resurvation to resturant.
+select date 
+select time 
+select number of guests (number of gusts is bigger then the max table)
+write telepone number / Email
+and click order</t>
+  </si>
+  <si>
+    <t>the Casual customer  want to make resurvation to resturant.
+select date 
+select time 
+select number of guests 
+write telepone number / Email
+and click order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+the DB is accessble
+there is table in that datetime in currect size </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the DB is accessble
+there is table in that datetime in currect size </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+the DB is accessble
+there is table empty 
+the number of goust bigger then the max size table
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+the DB is accessble
+there is table empty
+all the table in that size of order are already acupide by other Orders 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+after that the system get Ordering requsest for reserving table. The system check in the DB if there is table in that size 
+The system find that the there is no that big table in the resturant
+the system is sent responce to the sub that: "can't reserve palce to that much of people, you hit the limit of the biggest table (max 10)"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+after that the system get Ordering requsest for reserving table. The system check in the DB if date is valid 
+The system find that the date of ordering is too far, more then one month then the ordering moment:  isn't valid
+the system is sent responce to the sub that: "the time isn't correct cant order for this date. too far"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+after that the system get Ordering requsest for reserving table. The system check in the DB if time is valid 
+The system find that the time of oegring is less then the ordering moment:  isn't valid
+the system is sent responce to the sub that: "the time isn't correct cant order for this time. too close"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+after that the system get Ordering requsest for reserving table. The system check in the DB if time jump is valid 
+The system find that the time jump isn't valid
+the system is sent responce to the sub that: "the time jump isn't correct you can order only in  in hulf hour jump"
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+the GUI before sending Ordering request to the server check if all the fields was filled with data. 
+After the check the fields the GUI sent messege to the user that the "time field is emplty" </t>
+  </si>
+  <si>
+    <t>OrderSubscriberUnSuccessfulAuthFail</t>
+  </si>
+  <si>
+    <t>the subscriber give not valid auth infrmation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the subscriber is aleady in the system
+the DB is accessble
+</t>
+  </si>
+  <si>
+    <t>the system connect to DB to sub table and check if the auth of the subscriber is valid 
+the system find that the auth inforamtin is not correct.
+System sent messege: "the auth information is not right, check it and try again"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -196,8 +570,14 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,8 +602,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -246,13 +632,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -277,6 +678,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -614,10 +1033,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{527762F5-D11B-D449-919A-74259918E4FE}">
-  <dimension ref="A1:D38"/>
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="239" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A40" zoomScale="239" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="43.5" defaultRowHeight="73" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1046,6 +1468,376 @@
         <v>38</v>
       </c>
     </row>
+    <row r="39" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E9F4647-D5DC-FE4A-A219-07EADED0C61D}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="44.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="10" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="21.5" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="187" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="187" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="204" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="187" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="221" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="187" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="221" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding accetance test for reports of time
</commit_message>
<xml_diff>
--- a/system design/G16_Acceptance.xlsx
+++ b/system design/G16_Acceptance.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreibeloziorove/Desktop/middleProjectBistro_16/system design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A18E89D-0190-254C-B58D-565699814E5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C3C1AA-C536-6C40-80FA-2A82D8383DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="820" windowWidth="67260" windowHeight="27780" activeTab="1" xr2:uid="{DACF97BE-494E-BD4D-8128-8A3419E5BFA1}"/>
+    <workbookView xWindow="1340" yWindow="820" windowWidth="67260" windowHeight="27780" activeTab="2" xr2:uid="{DACF97BE-494E-BD4D-8128-8A3419E5BFA1}"/>
   </bookViews>
   <sheets>
     <sheet name="requirments" sheetId="1" r:id="rId1"/>
     <sheet name="Acceptence test Ordering " sheetId="2" r:id="rId2"/>
+    <sheet name="Acceptance test time report" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="130">
   <si>
     <t>The system will allow you to register subscribers to the system</t>
   </si>
@@ -536,6 +537,67 @@
     <t>the system connect to DB to sub table and check if the auth of the subscriber is valid 
 the system find that the auth inforamtin is not correct.
 System sent messege: "the auth information is not right, check it and try again"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the maneger want to see the time report 
+he enter to  GUI and 
+enter 
+valid datetime to start the report
+valid datetime to end the report
+end click enter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">the system enter the the database and get all the informatin of the Orders and queue form the db 
+the system analize the data.
+Split it to how much was make orders, and how mush was enter the queue
+how much from the orders was late 
+the system make report of it with grafics and sent it as a result to the manager </t>
+  </si>
+  <si>
+    <t>the server is accisble 
+the DB is accesable 
+the data of the Orders in that time range aviable
+the data of the Queue in that time range aviable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the manager want to see report about the orders time and about the queue times
+the system get to the report </t>
+  </si>
+  <si>
+    <t>reportWithDataSusssesful</t>
+  </si>
+  <si>
+    <t>reportWithoutDataFail</t>
+  </si>
+  <si>
+    <t>the system enter the the database and get all the informatin of the Orders and queue form the db 
+the system find that there no data in that time range and sent messege : "data not found for this range"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the server is accisble 
+the DB is accesable 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the manager want to see report about the orders time and about the queue times
+the system cant find data on this time range
+the system get to the report </t>
+  </si>
+  <si>
+    <t>reportWithoutDateTimeFail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the maneger want to see the time report 
+he enter to  GUI and 
+enter 
+valid datetime to end the report
+end click enter </t>
+  </si>
+  <si>
+    <t>the GUI check if all the fuilds are full. The system write massege that need to fill the datetime to start report</t>
+  </si>
+  <si>
+    <t>the manager want to see report about, but forget to fill all the fields so ther GUI will tell them that</t>
   </si>
 </sst>
 </file>
@@ -1535,8 +1597,8 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="400" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="90" zoomScaleNormal="400" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1841,4 +1903,97 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020A0F01-E653-8E4D-8DA1-C72F8EC07905}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="194" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="50" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding acceptance test for table clear
</commit_message>
<xml_diff>
--- a/system design/G16_Acceptance.xlsx
+++ b/system design/G16_Acceptance.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreibeloziorove/Desktop/middleProjectBistro_16/system design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Studies\MidProject\Requirements\middleProjectBistro_16\system design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C3C1AA-C536-6C40-80FA-2A82D8383DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61EDB20-D952-45C2-B720-633CAD7D425D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="820" windowWidth="67260" windowHeight="27780" activeTab="2" xr2:uid="{DACF97BE-494E-BD4D-8128-8A3419E5BFA1}"/>
+    <workbookView xWindow="6915" yWindow="1470" windowWidth="14010" windowHeight="10875" activeTab="3" xr2:uid="{DACF97BE-494E-BD4D-8128-8A3419E5BFA1}"/>
   </bookViews>
   <sheets>
     <sheet name="requirments" sheetId="1" r:id="rId1"/>
     <sheet name="Acceptence test Ordering " sheetId="2" r:id="rId2"/>
     <sheet name="Acceptance test time report" sheetId="3" r:id="rId3"/>
+    <sheet name="Acceptance test table clear" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="151">
   <si>
     <t>The system will allow you to register subscribers to the system</t>
   </si>
@@ -599,30 +600,121 @@
   <si>
     <t>the manager want to see report about, but forget to fill all the fields so ther GUI will tell them that</t>
   </si>
+  <si>
+    <t>FailToClearTableWrongCode</t>
+  </si>
+  <si>
+    <t>Costumer ask for the bill or log in through the terminal
+System procure bill for the costumer based on his status Subscriber or Guest
+Costumer insert WRONG confirmation code
+System procure message "Wrong confirmation code"</t>
+  </si>
+  <si>
+    <t>Current table has not been payed
+wrong confirmation code given
+Table could not be cleared</t>
+  </si>
+  <si>
+    <t>FailToClearTableEmptyCode</t>
+  </si>
+  <si>
+    <t>Costumer ask for the bill or log in through the terminal
+System procure bill for the costumer based on his status Subscriber or Guest
+Costumer insert Empty confirmation code
+System procure message "Wrong confirmation code"</t>
+  </si>
+  <si>
+    <t>FailToClearTablePaymentFailed</t>
+  </si>
+  <si>
+    <t>Costumer ask for the bill or log in through the terminal
+Costumer insert Correct confirmation code
+Costumer tries to pay his bill
+System check wether Payment occured</t>
+  </si>
+  <si>
+    <t>Payment failed
+Table could not be cleared</t>
+  </si>
+  <si>
+    <t>TableClearedSuccessfullly</t>
+  </si>
+  <si>
+    <t>Costumer ask for the bill or log in through the terminal
+System procure bill for the costumer based on his status Subscriber or Guest
+Costumer insert Correct confirmation code
+Costumer tries to pay his bill
+System check wether Payment occurred</t>
+  </si>
+  <si>
+    <t>Payment Succeded
+Table Cleared Successfullly</t>
+  </si>
+  <si>
+    <t>BillDiscountTest</t>
+  </si>
+  <si>
+    <t>Costumer ask for the bill
+System procure bill for the costumer based on his status Subscriber or Guest
+System recognize it is a Subscriber
+System procures bill with 10% discount
+Costumer insert Correct confirmation code
+Costumer tries to pay his bill
+System check wether Payment occurred</t>
+  </si>
+  <si>
+    <t>Costumer is a subscriber</t>
+  </si>
+  <si>
+    <t>SystemBillMessageFailCanceledTable</t>
+  </si>
+  <si>
+    <t>System recognize two hours
+System  try to procure bill for the costumer based on his status Subscriber or Guest
+System could not create the bill</t>
+  </si>
+  <si>
+    <t>Bill could not be made.
+Table canceled</t>
+  </si>
+  <si>
+    <t>Two Hours Passed</t>
+  </si>
+  <si>
+    <t>SystemBillMessageSuccess</t>
+  </si>
+  <si>
+    <t>System recognize two hours
+System try to procure bill for the costumer based on his status Subscriber or Guest
+System sends bill to costumer</t>
+  </si>
+  <si>
+    <t>Bill Sent to costumer</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -715,7 +807,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -759,10 +851,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
+    <cellStyle name="40% - הדגשה1" xfId="1" builtinId="31"/>
+    <cellStyle name="60% - הדגשה2" xfId="2" builtinId="36"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -779,7 +874,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1104,13 +1199,13 @@
       <selection activeCell="A43" sqref="A43:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="43.5" defaultRowHeight="73" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="43.44140625" defaultRowHeight="72.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="43.5" style="1"/>
+    <col min="2" max="16384" width="43.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="72.95" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
@@ -1121,7 +1216,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="72.95" customHeight="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1133,7 +1228,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="72.95" customHeight="1">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1145,7 +1240,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="72.95" customHeight="1">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1156,7 +1251,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="72.95" customHeight="1">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1167,7 +1262,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="72.95" customHeight="1">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1178,7 +1273,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="72.95" customHeight="1">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1189,7 +1284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="72.95" customHeight="1">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1200,7 +1295,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="72.95" customHeight="1">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1211,7 +1306,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="72.95" customHeight="1">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1222,7 +1317,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="72.95" customHeight="1">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1233,7 +1328,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="72.95" customHeight="1">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1244,7 +1339,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="72.95" customHeight="1">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1255,7 +1350,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="72.95" customHeight="1">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1266,7 +1361,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="72.95" customHeight="1">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1277,7 +1372,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="72.95" customHeight="1">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1288,7 +1383,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="72.95" customHeight="1">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1299,7 +1394,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="72.95" customHeight="1">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1310,7 +1405,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="72.95" customHeight="1">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1321,7 +1416,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="72.95" customHeight="1">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1332,7 +1427,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="72.95" customHeight="1">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1343,7 +1438,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="72.95" customHeight="1">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1354,7 +1449,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="72.95" customHeight="1">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1365,7 +1460,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="72.95" customHeight="1">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1376,7 +1471,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="72.95" customHeight="1">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1387,7 +1482,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="72.95" customHeight="1">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1398,7 +1493,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="72.95" customHeight="1">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1409,7 +1504,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="72.95" customHeight="1">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1420,7 +1515,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="72.95" customHeight="1">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1431,7 +1526,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="72.95" customHeight="1">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1442,7 +1537,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="72.95" customHeight="1">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1453,7 +1548,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="72.95" customHeight="1">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1464,7 +1559,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="72.95" customHeight="1">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1475,7 +1570,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="72.95" customHeight="1">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1486,7 +1581,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="72.95" customHeight="1">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1497,7 +1592,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="72.95" customHeight="1">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1508,7 +1603,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="72.95" customHeight="1">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1519,7 +1614,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="72.95" customHeight="1">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1530,7 +1625,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="72.95" customHeight="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1541,7 +1636,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="72.95" customHeight="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1552,7 +1647,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="72.95" customHeight="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1563,7 +1658,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="72.95" customHeight="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1574,7 +1669,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="72.95" customHeight="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1601,17 +1696,17 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="44.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="37.83203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="37.77734375" style="10" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="21.5" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="10"/>
+    <col min="5" max="5" width="21.44140625" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="10.77734375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
@@ -1628,7 +1723,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="135">
       <c r="A2" s="11" t="s">
         <v>49</v>
       </c>
@@ -1645,7 +1740,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="187" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="165">
       <c r="A3" s="11" t="s">
         <v>54</v>
       </c>
@@ -1662,7 +1757,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="120">
       <c r="A4" s="11" t="s">
         <v>64</v>
       </c>
@@ -1679,7 +1774,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="150">
       <c r="A5" s="11" t="s">
         <v>69</v>
       </c>
@@ -1696,7 +1791,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="187" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="165">
       <c r="A6" s="11" t="s">
         <v>70</v>
       </c>
@@ -1713,7 +1808,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="204" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="180">
       <c r="A7" s="11" t="s">
         <v>75</v>
       </c>
@@ -1730,7 +1825,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="187" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="165">
       <c r="A8" s="11" t="s">
         <v>79</v>
       </c>
@@ -1747,7 +1842,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="221" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="180">
       <c r="A9" s="11" t="s">
         <v>83</v>
       </c>
@@ -1764,7 +1859,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="120">
       <c r="A10" s="11" t="s">
         <v>89</v>
       </c>
@@ -1781,7 +1876,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="105">
       <c r="A11" s="11" t="s">
         <v>90</v>
       </c>
@@ -1798,7 +1893,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="135">
       <c r="A12" s="11" t="s">
         <v>91</v>
       </c>
@@ -1815,7 +1910,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="150">
       <c r="A13" s="11" t="s">
         <v>92</v>
       </c>
@@ -1832,7 +1927,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="187" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="165">
       <c r="A14" s="11" t="s">
         <v>93</v>
       </c>
@@ -1849,7 +1944,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="170" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="150">
       <c r="A15" s="11" t="s">
         <v>94</v>
       </c>
@@ -1866,7 +1961,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="221" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="180">
       <c r="A16" s="11" t="s">
         <v>95</v>
       </c>
@@ -1883,7 +1978,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="105">
       <c r="A17" s="11" t="s">
         <v>113</v>
       </c>
@@ -1912,20 +2007,20 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="194" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.1640625" customWidth="1"/>
+    <col min="1" max="1" width="36.109375" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" customWidth="1"/>
+    <col min="4" max="4" width="28.109375" customWidth="1"/>
     <col min="5" max="5" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
@@ -1942,7 +2037,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="136" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="120">
       <c r="A2" s="11" t="s">
         <v>121</v>
       </c>
@@ -1959,7 +2054,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="105">
       <c r="A3" s="11" t="s">
         <v>122</v>
       </c>
@@ -1976,7 +2071,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="90">
       <c r="A4" s="11" t="s">
         <v>126</v>
       </c>
@@ -1991,6 +2086,130 @@
       </c>
       <c r="E4" s="12" t="s">
         <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8688B799-49D1-4918-AA0D-93A22290DA03}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.21875" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="390">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="390">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="315">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="409.5">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="409.5">
+      <c r="A6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="240">
+      <c r="A7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="240">
+      <c r="A8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Getting Table Acceptance Test
</commit_message>
<xml_diff>
--- a/system design/G16_Acceptance.xlsx
+++ b/system design/G16_Acceptance.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Studies\MidProject\Requirements\middleProjectBistro_16\system design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asafeliyahu/git/repository/middleProjectBistro_16/system design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61EDB20-D952-45C2-B720-633CAD7D425D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628F1A63-7C63-9B48-BF89-BDD031DCCAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="1470" windowWidth="14010" windowHeight="10875" activeTab="3" xr2:uid="{DACF97BE-494E-BD4D-8128-8A3419E5BFA1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" firstSheet="2" activeTab="3" xr2:uid="{DACF97BE-494E-BD4D-8128-8A3419E5BFA1}"/>
   </bookViews>
   <sheets>
     <sheet name="requirments" sheetId="1" r:id="rId1"/>
     <sheet name="Acceptence test Ordering " sheetId="2" r:id="rId2"/>
     <sheet name="Acceptance test time report" sheetId="3" r:id="rId3"/>
     <sheet name="Acceptance test table clear" sheetId="4" r:id="rId4"/>
+    <sheet name="Acceptance Test Getting Table" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="179">
   <si>
     <t>The system will allow you to register subscribers to the system</t>
   </si>
@@ -691,30 +692,199 @@
   <si>
     <t>Bill Sent to costumer</t>
   </si>
+  <si>
+    <t>SubscriberIndentifyWithQRCodeSuccess</t>
+  </si>
+  <si>
+    <t>The subscriber arrived to the resutrant
+Subscriber's order arrived or table is available for subscriber
+Subscriber shows his QRCode to the QRCode reader</t>
+  </si>
+  <si>
+    <t>System received QRCode from the Subscriber
+System access to the DB
+System will attempt to find the Subscriber in the DB
+System will attempt to find the Subscriber's order in the DB
+System has found the Subscriber's order in the DB
+System successfully validated the subscriber's order
+System will alert the Subscriber that the identfication was successfull</t>
+  </si>
+  <si>
+    <t>The restaurant is open
+Server is available
+Database is accessiable
+The guest is a subscriber
+The subscriber has a valid order (meaning it is the order time or there is an available table)
+The Subscriber's QRCode is valid</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>SubscriberIndentifyWithQRCodeFailed</t>
+  </si>
+  <si>
+    <t>The subscriber arrived to the resutrant
+Subscriber shows his QRCode to the QRCode reader</t>
+  </si>
+  <si>
+    <t>System received QRCode from the Subscriber
+System access to the DB
+System will attempt to find the Subscriber in the DB
+System will attempt to find the Subscriber's order in the DB
+System has found that the subscriber's order time is not yet arrived
+System will display a messsage "You have arrived early please wait untill your order time arrived"</t>
+  </si>
+  <si>
+    <t>The restaurant is open
+Server is available
+Database is accessiable
+The guest is a subscriber
+The subscriber has a valid order
+The Subscriber's QRCode is valid
+The subscriber has tried to indetify before his order time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This test will check if the subscriber tries to indetify when his order time has not yet arrived </t>
+  </si>
+  <si>
+    <t>GuestEntertedCorrectAcceptenceCode</t>
+  </si>
+  <si>
+    <t>The Guest has arrived to the restaurant's terminal
+Guest's order arrived or table is available for subscriber
+The Guest has enterted his order's acceptence code
+The Guest has clicked on "verify"</t>
+  </si>
+  <si>
+    <t>System has recived guest's order acceptence code
+System access to the DB
+System will attempt to find the guest's order with the acceptence code
+System will validate the guest's order (order time)
+System will verify the guest's acceptence code
+System successfully verfied the guest's acceptence code
+Systme will display a message to the guest's "Verfication successful, have a good dinning."</t>
+  </si>
+  <si>
+    <t>SubscriberEntertedCorrectAcceptenceCode</t>
+  </si>
+  <si>
+    <t>The subsriber has arrived to the restaurant's terminal
+Subscriber's order arrived or table is available for subscriber
+The subscriber has enterted his order's acceptence code
+The subscriber has clicked on "verify"</t>
+  </si>
+  <si>
+    <t>System has recived subscriber's order acceptence code
+System access to the DB
+System will attempt to find the subscriber in the DB
+System successfully found the subscriber in the DB
+System will attempt to find the subscriber's order
+System will validate the subscriber's order (order time)
+System will verify the subscriber's acceptence code
+System successfully verfied the subscriber's acceptence code
+Systme will display a message to the subscriber "Verfication successful, have a good dinning."</t>
+  </si>
+  <si>
+    <t>The restaurant is open
+Server is available
+Database is accessiable
+The guest is a subscriber
+The subscriber has a valid order (order time)
+The Subscriber's acceptence code is valid</t>
+  </si>
+  <si>
+    <t>SubscriberEntertedIncorrectAcceptenceCode</t>
+  </si>
+  <si>
+    <t>System has recived subscriber's order acceptence code
+System access to the DB
+System will attempt to find the subscriber in the DB
+System successfully found the subscriber in the DB
+System will attempt to find the subscriber's order
+System will validate the subscriber's order (order time)
+System will verify the subscriber's acceptence code
+System failed  verfied the subscriber's acceptence code
+Systme will display a message to the subscriber "Verfication failed, please enter your order correct acceptence code."</t>
+  </si>
+  <si>
+    <t>The restaurant is open
+Server is available
+Database is accessiable
+The guest is a subscriber
+The subscriber has a valid order (order time)
+The Subscriber's acceptence code is incorrect</t>
+  </si>
+  <si>
+    <t>SubscriberEntertedEmpryAcceptenceCode</t>
+  </si>
+  <si>
+    <t>The subsriber has arrived to the restaurant's terminal
+Subscriber's order arrived or table is available for subscriber
+The subscriber has clicked on "verify"</t>
+  </si>
+  <si>
+    <t>System has recived subscriber's order acceptence code
+System will display a message to the subscriber "No acceptence code has entered, please enter your order's acceptence code</t>
+  </si>
+  <si>
+    <t>The restaurant is open
+Server is available
+Database is accessiable
+The guest is a subscriber
+The subscriber has a valid order (order time)
+The Subscriber's aentered an empty acceptence code</t>
+  </si>
+  <si>
+    <t>GuestRecievedCodeAcceptenceAfterClickedLostMyCode</t>
+  </si>
+  <si>
+    <t>The guest has arrived to the resturant
+guest's order is valid or table is available for guest
+The guest clicks on Lost My Code</t>
+  </si>
+  <si>
+    <t>System displays a form to the guest
+The guest enteres his email and phone number
+The guest clicks on OK
+The system will access the DB
+The system will attempt to find the guest's order with the email and phone number
+System successfully found the guest's order
+The system will send to the guest via email and SMS the Acceptence Code
+System will display a message in the terminal to the guest that "Acceptence Code successfully restored"</t>
+  </si>
+  <si>
+    <t>The guest is in the resturant
+The resturant is opened
+Server is available
+Server is accessiable
+The guest has a valid order
+The guest has a valid email and phone number</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -730,8 +900,29 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -762,8 +953,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -801,13 +998,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -854,10 +1064,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="40% - הדגשה1" xfId="1" builtinId="31"/>
-    <cellStyle name="60% - הדגשה2" xfId="2" builtinId="36"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1199,13 +1427,13 @@
       <selection activeCell="A43" sqref="A43:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="43.44140625" defaultRowHeight="72.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="43.5" defaultRowHeight="73" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="43.44140625" style="1"/>
+    <col min="2" max="16384" width="43.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="72.95" customHeight="1">
+    <row r="1" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
@@ -1216,7 +1444,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="72.95" customHeight="1">
+    <row r="2" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1228,7 +1456,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="72.95" customHeight="1">
+    <row r="3" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1240,7 +1468,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="72.95" customHeight="1">
+    <row r="4" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1251,7 +1479,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="72.95" customHeight="1">
+    <row r="5" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1262,7 +1490,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="72.95" customHeight="1">
+    <row r="6" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1273,7 +1501,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="72.95" customHeight="1">
+    <row r="7" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1284,7 +1512,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="72.95" customHeight="1">
+    <row r="8" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1295,7 +1523,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="72.95" customHeight="1">
+    <row r="9" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1306,7 +1534,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="72.95" customHeight="1">
+    <row r="10" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1317,7 +1545,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="72.95" customHeight="1">
+    <row r="11" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1328,7 +1556,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="72.95" customHeight="1">
+    <row r="12" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1339,7 +1567,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="72.95" customHeight="1">
+    <row r="13" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1350,7 +1578,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="72.95" customHeight="1">
+    <row r="14" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1361,7 +1589,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="72.95" customHeight="1">
+    <row r="15" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1372,7 +1600,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="72.95" customHeight="1">
+    <row r="16" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1383,7 +1611,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="72.95" customHeight="1">
+    <row r="17" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1394,7 +1622,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="72.95" customHeight="1">
+    <row r="18" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1405,7 +1633,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="72.95" customHeight="1">
+    <row r="19" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1416,7 +1644,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="72.95" customHeight="1">
+    <row r="20" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1427,7 +1655,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="72.95" customHeight="1">
+    <row r="21" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1438,7 +1666,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="72.95" customHeight="1">
+    <row r="22" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1449,7 +1677,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="72.95" customHeight="1">
+    <row r="23" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1460,7 +1688,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="72.95" customHeight="1">
+    <row r="24" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1471,7 +1699,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="72.95" customHeight="1">
+    <row r="25" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1482,7 +1710,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="72.95" customHeight="1">
+    <row r="26" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1493,7 +1721,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="72.95" customHeight="1">
+    <row r="27" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1504,7 +1732,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="72.95" customHeight="1">
+    <row r="28" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1515,7 +1743,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="72.95" customHeight="1">
+    <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1526,7 +1754,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="72.95" customHeight="1">
+    <row r="30" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1537,7 +1765,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="72.95" customHeight="1">
+    <row r="31" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1548,7 +1776,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="72.95" customHeight="1">
+    <row r="32" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1559,7 +1787,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="72.95" customHeight="1">
+    <row r="33" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1570,7 +1798,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="72.95" customHeight="1">
+    <row r="34" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1581,7 +1809,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="72.95" customHeight="1">
+    <row r="35" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1592,7 +1820,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="72.95" customHeight="1">
+    <row r="36" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1603,7 +1831,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="72.95" customHeight="1">
+    <row r="37" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1614,7 +1842,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="72.95" customHeight="1">
+    <row r="38" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1625,7 +1853,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="72.95" customHeight="1">
+    <row r="39" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1636,7 +1864,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="72.95" customHeight="1">
+    <row r="40" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1647,7 +1875,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="72.95" customHeight="1">
+    <row r="41" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1658,7 +1886,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="72.95" customHeight="1">
+    <row r="42" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1669,7 +1897,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="72.95" customHeight="1">
+    <row r="43" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1696,17 +1924,17 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="44.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="37.77734375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="33.5" style="10" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" style="10" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="21.44140625" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="10.77734375" style="10"/>
+    <col min="5" max="5" width="21.5" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
@@ -1723,7 +1951,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="135">
+    <row r="2" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>49</v>
       </c>
@@ -1740,7 +1968,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="165">
+    <row r="3" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>54</v>
       </c>
@@ -1757,7 +1985,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="120">
+    <row r="4" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>64</v>
       </c>
@@ -1774,7 +2002,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="150">
+    <row r="5" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>69</v>
       </c>
@@ -1791,7 +2019,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="165">
+    <row r="6" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>70</v>
       </c>
@@ -1808,7 +2036,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="180">
+    <row r="7" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>75</v>
       </c>
@@ -1825,7 +2053,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="165">
+    <row r="8" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>79</v>
       </c>
@@ -1842,7 +2070,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="180">
+    <row r="9" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>83</v>
       </c>
@@ -1859,7 +2087,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="120">
+    <row r="10" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>89</v>
       </c>
@@ -1876,7 +2104,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="105">
+    <row r="11" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>90</v>
       </c>
@@ -1893,7 +2121,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="135">
+    <row r="12" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>91</v>
       </c>
@@ -1910,7 +2138,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="150">
+    <row r="13" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>92</v>
       </c>
@@ -1927,7 +2155,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="165">
+    <row r="14" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>93</v>
       </c>
@@ -1944,7 +2172,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="150">
+    <row r="15" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>94</v>
       </c>
@@ -1961,7 +2189,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="180">
+    <row r="16" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>95</v>
       </c>
@@ -1978,7 +2206,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="105">
+    <row r="17" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
         <v>113</v>
       </c>
@@ -2011,16 +2239,16 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.109375" customWidth="1"/>
+    <col min="1" max="1" width="36.1640625" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="28.109375" customWidth="1"/>
+    <col min="4" max="4" width="28.1640625" customWidth="1"/>
     <col min="5" max="5" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
@@ -2037,7 +2265,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="120">
+    <row r="2" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>121</v>
       </c>
@@ -2054,7 +2282,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="105">
+    <row r="3" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
         <v>122</v>
       </c>
@@ -2071,7 +2299,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="90">
+    <row r="4" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
         <v>126</v>
       </c>
@@ -2095,121 +2323,283 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8688B799-49D1-4918-AA0D-93A22290DA03}">
+  <sheetPr>
+    <tabColor theme="8" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="176" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="224" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>144</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CC20D7F-024B-D348-AC62-F023D117519D}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
+    <col min="3" max="3" width="39.83203125" customWidth="1"/>
+    <col min="4" max="4" width="38.5" customWidth="1"/>
+    <col min="5" max="5" width="79.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="17" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="390">
-      <c r="A2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="390">
-      <c r="A3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="315">
-      <c r="A4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="409.5">
-      <c r="A5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="409.5">
-      <c r="A6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="240">
-      <c r="A7" t="s">
-        <v>144</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="240">
-      <c r="A8" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="D8" t="s">
-        <v>147</v>
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A2" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="320" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Preconditions to Acceptance test Clear Table
</commit_message>
<xml_diff>
--- a/system design/G16_Acceptance.xlsx
+++ b/system design/G16_Acceptance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asafeliyahu/git/repository/middleProjectBistro_16/system design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Studies\MidProject\Requirements\middleProjectBistro_16\system design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628F1A63-7C63-9B48-BF89-BDD031DCCAA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52A52D1-9FE7-4D65-BACB-714C53D1AB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" firstSheet="2" activeTab="3" xr2:uid="{DACF97BE-494E-BD4D-8128-8A3419E5BFA1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16080" firstSheet="2" activeTab="3" xr2:uid="{DACF97BE-494E-BD4D-8128-8A3419E5BFA1}"/>
   </bookViews>
   <sheets>
     <sheet name="requirments" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="180">
   <si>
     <t>The system will allow you to register subscribers to the system</t>
   </si>
@@ -861,30 +861,36 @@
 The guest has a valid order
 The guest has a valid email and phone number</t>
   </si>
+  <si>
+    <t>Database is accessable
+System can verify confirmation codes
+Payment system works as expected
+Table is not canceled or cleared already</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1084,8 +1090,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="60% - Accent2" xfId="2" builtinId="36"/>
+    <cellStyle name="40% - הדגשה1" xfId="1" builtinId="31"/>
+    <cellStyle name="60% - הדגשה2" xfId="2" builtinId="36"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1427,13 +1433,13 @@
       <selection activeCell="A43" sqref="A43:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="43.5" defaultRowHeight="73" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="43.44140625" defaultRowHeight="72.95" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="43.5" style="1"/>
+    <col min="2" max="16384" width="43.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="72.95" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>34</v>
       </c>
@@ -1444,7 +1450,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="72.95" customHeight="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1456,7 +1462,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="72.95" customHeight="1">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -1468,7 +1474,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="72.95" customHeight="1">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -1479,7 +1485,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="72.95" customHeight="1">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1490,7 +1496,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="72.95" customHeight="1">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -1501,7 +1507,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="72.95" customHeight="1">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -1512,7 +1518,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="72.95" customHeight="1">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -1523,7 +1529,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="72.95" customHeight="1">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -1534,7 +1540,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="72.95" customHeight="1">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -1545,7 +1551,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="72.95" customHeight="1">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1556,7 +1562,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="72.95" customHeight="1">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1567,7 +1573,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="72.95" customHeight="1">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1578,7 +1584,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="72.95" customHeight="1">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1589,7 +1595,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="72.95" customHeight="1">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1600,7 +1606,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="72.95" customHeight="1">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1611,7 +1617,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="72.95" customHeight="1">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1622,7 +1628,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="72.95" customHeight="1">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1633,7 +1639,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="72.95" customHeight="1">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1644,7 +1650,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="72.95" customHeight="1">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1655,7 +1661,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="72.95" customHeight="1">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1666,7 +1672,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="72.95" customHeight="1">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1677,7 +1683,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="72.95" customHeight="1">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1688,7 +1694,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="72.95" customHeight="1">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1699,7 +1705,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="72.95" customHeight="1">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1710,7 +1716,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="72.95" customHeight="1">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1721,7 +1727,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="72.95" customHeight="1">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1732,7 +1738,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="72.95" customHeight="1">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1743,7 +1749,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="72.95" customHeight="1">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1754,7 +1760,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="72.95" customHeight="1">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1765,7 +1771,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="72.95" customHeight="1">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1776,7 +1782,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="72.95" customHeight="1">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1787,7 +1793,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="72.95" customHeight="1">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="72.95" customHeight="1">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1809,7 +1815,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="72.95" customHeight="1">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1820,7 +1826,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="72.95" customHeight="1">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="72.95" customHeight="1">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -1842,7 +1848,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="72.95" customHeight="1">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -1853,7 +1859,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="72.95" customHeight="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1864,7 +1870,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="72.95" customHeight="1">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1875,7 +1881,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="72.95" customHeight="1">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1886,7 +1892,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" ht="72.95" customHeight="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1897,7 +1903,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" ht="72.95" customHeight="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1924,17 +1930,17 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="44.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5" style="10" customWidth="1"/>
-    <col min="3" max="3" width="37.83203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="33.44140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="37.77734375" style="10" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="21.5" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="10"/>
+    <col min="5" max="5" width="21.44140625" style="10" customWidth="1"/>
+    <col min="6" max="16384" width="10.77734375" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
@@ -1951,7 +1957,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="135">
       <c r="A2" s="11" t="s">
         <v>49</v>
       </c>
@@ -1968,7 +1974,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="176" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="165">
       <c r="A3" s="11" t="s">
         <v>54</v>
       </c>
@@ -1985,7 +1991,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="120">
       <c r="A4" s="11" t="s">
         <v>64</v>
       </c>
@@ -2002,7 +2008,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="150">
       <c r="A5" s="11" t="s">
         <v>69</v>
       </c>
@@ -2019,7 +2025,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="176" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="165">
       <c r="A6" s="11" t="s">
         <v>70</v>
       </c>
@@ -2036,7 +2042,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="192" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="180">
       <c r="A7" s="11" t="s">
         <v>75</v>
       </c>
@@ -2053,7 +2059,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="176" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="165">
       <c r="A8" s="11" t="s">
         <v>79</v>
       </c>
@@ -2070,7 +2076,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="208" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="180">
       <c r="A9" s="11" t="s">
         <v>83</v>
       </c>
@@ -2087,7 +2093,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="120">
       <c r="A10" s="11" t="s">
         <v>89</v>
       </c>
@@ -2104,7 +2110,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="105">
       <c r="A11" s="11" t="s">
         <v>90</v>
       </c>
@@ -2121,7 +2127,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="135">
       <c r="A12" s="11" t="s">
         <v>91</v>
       </c>
@@ -2138,7 +2144,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="150">
       <c r="A13" s="11" t="s">
         <v>92</v>
       </c>
@@ -2155,7 +2161,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="176" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="165">
       <c r="A14" s="11" t="s">
         <v>93</v>
       </c>
@@ -2172,7 +2178,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="150">
       <c r="A15" s="11" t="s">
         <v>94</v>
       </c>
@@ -2189,7 +2195,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="208" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="180">
       <c r="A16" s="11" t="s">
         <v>95</v>
       </c>
@@ -2206,7 +2212,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="105">
       <c r="A17" s="11" t="s">
         <v>113</v>
       </c>
@@ -2239,16 +2245,16 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.1640625" customWidth="1"/>
+    <col min="1" max="1" width="36.109375" customWidth="1"/>
     <col min="2" max="2" width="32.33203125" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" customWidth="1"/>
+    <col min="4" max="4" width="28.109375" customWidth="1"/>
     <col min="5" max="5" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>42</v>
       </c>
@@ -2265,7 +2271,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="120">
       <c r="A2" s="11" t="s">
         <v>121</v>
       </c>
@@ -2282,7 +2288,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="105">
       <c r="A3" s="11" t="s">
         <v>122</v>
       </c>
@@ -2299,7 +2305,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="90">
       <c r="A4" s="11" t="s">
         <v>126</v>
       </c>
@@ -2328,19 +2334,20 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" customWidth="1"/>
-    <col min="4" max="4" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
+    <col min="3" max="3" width="26.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -2357,7 +2364,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="135">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -2367,8 +2374,11 @@
       <c r="C2" s="15" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+      <c r="D2" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="135">
       <c r="A3" t="s">
         <v>133</v>
       </c>
@@ -2378,8 +2388,11 @@
       <c r="C3" s="15" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+      <c r="D3" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="105">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -2389,8 +2402,11 @@
       <c r="C4" s="15" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="176" x14ac:dyDescent="0.2">
+      <c r="D4" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="150">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -2400,8 +2416,11 @@
       <c r="C5" s="15" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="224" x14ac:dyDescent="0.2">
+      <c r="D5" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="195">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -2415,7 +2434,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="90">
       <c r="A7" t="s">
         <v>144</v>
       </c>
@@ -2429,7 +2448,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="128" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="90">
       <c r="A8" t="s">
         <v>148</v>
       </c>
@@ -2455,20 +2474,20 @@
   </sheetPr>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" customWidth="1"/>
-    <col min="3" max="3" width="39.83203125" customWidth="1"/>
-    <col min="4" max="4" width="38.5" customWidth="1"/>
+    <col min="2" max="2" width="34.77734375" customWidth="1"/>
+    <col min="3" max="3" width="39.77734375" customWidth="1"/>
+    <col min="4" max="4" width="38.44140625" customWidth="1"/>
     <col min="5" max="5" width="79.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1">
       <c r="A1" s="16" t="s">
         <v>42</v>
       </c>
@@ -2485,7 +2504,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="173.25">
       <c r="A2" s="18" t="s">
         <v>151</v>
       </c>
@@ -2502,7 +2521,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="157.5">
       <c r="A3" s="18" t="s">
         <v>156</v>
       </c>
@@ -2519,7 +2538,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="150">
       <c r="A4" s="18" t="s">
         <v>161</v>
       </c>
@@ -2534,7 +2553,7 @@
       </c>
       <c r="E4" s="18"/>
     </row>
-    <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="165">
       <c r="A5" s="18" t="s">
         <v>164</v>
       </c>
@@ -2551,7 +2570,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="165">
       <c r="A6" s="18" t="s">
         <v>168</v>
       </c>
@@ -2568,7 +2587,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="320" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="90">
       <c r="A7" s="18" t="s">
         <v>171</v>
       </c>
@@ -2585,7 +2604,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="165">
       <c r="A8" s="18" t="s">
         <v>175</v>
       </c>

</xml_diff>